<commit_message>
modelisation : update of tables. Documentation : descriptions of some tables and fields and list of questions.
</commit_message>
<xml_diff>
--- a/Documentation/database-tables.xlsx
+++ b/Documentation/database-tables.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clem\01-coding-projects\08-sql-projects\projet-bdd-2021\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8A099D-A10E-4A19-B65E-2C22ADC25160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6861F8A1-7EBC-4D0A-BD78-08D7D0C9F5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D0EBE73F-8EE6-4ABE-837B-C7604514A6B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D0EBE73F-8EE6-4ABE-837B-C7604514A6B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Modélisation" sheetId="1" r:id="rId1"/>
     <sheet name="Agents" sheetId="4" r:id="rId2"/>
     <sheet name="Règle" sheetId="2" r:id="rId3"/>
-    <sheet name="Remarques" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -344,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
   <si>
     <t>BDD</t>
   </si>
@@ -367,9 +366,6 @@
     <t>jazz, blues, classique, rock, …</t>
   </si>
   <si>
-    <t>Ŕealisations precedentes : films realises, pieces de theatre ou spectacles mis en scene, roles joues dans les films et au theatre, les albums (pour les musiciens)</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -388,9 +384,6 @@
     <t>Le Monde, blog, …</t>
   </si>
   <si>
-    <t>Pour un film dans lequel a joué une actrice de l'agence, il serait intéressant d'indiquer dans les infos du film qui en est la réalistrice. Mais pas pour un film qui a été dirigé par une réalisatrice de l'agence. Comment faire ? Simplement ne pas indiquer la réalisatrice ?</t>
-  </si>
-  <si>
     <t>pas d'accent</t>
   </si>
   <si>
@@ -689,45 +682,6 @@
   </si>
   <si>
     <t>text contenant prix, date, œuvre, etc.</t>
-  </si>
-  <si>
-    <t>Questions</t>
-  </si>
-  <si>
-    <t>Est-ce problématique d'avoir une table où des infos se répettent ?</t>
-  </si>
-  <si>
-    <t>Une solution simple est de ne pas répéter les info et de faire une table pour faire la jointure</t>
-  </si>
-  <si>
-    <t>Par exemple des tables : skills, artists, et une table de jointure entre les 2</t>
-  </si>
-  <si>
-    <t>Dans la table Trainings</t>
-  </si>
-  <si>
-    <t>Les info se répètent si 2 artistes ont la même formation. Mais il y a peu d'info donc ce n'est pas très grave et ça permet de ne pas avoir à faire une table supplémentaire pour lier artiste et training.</t>
-  </si>
-  <si>
-    <t>Table Artist</t>
-  </si>
-  <si>
-    <t>Awards, Review, festivals sont des zones de texte avec toutes les info dedans. Permet de ne pas multiplier le nombre de tables</t>
-  </si>
-  <si>
-    <t>Table creation</t>
-  </si>
-  <si>
-    <t>attribut type : album_written, album_produced, album_sung, film_produced, etc.</t>
-  </si>
-  <si>
-    <t>suivi de id_artist</t>
-  </si>
-  <si>
-    <t>Le but est de ne pas avoir une table en plus faisant le lien entre artist et creation</t>
-  </si>
-  <si>
-    <t>Mais la meilleure solution serait d'avoir cette table faisant le lien (et seulement album, film, etc. pour les types) car sinon des infos vont se répéter + il va y avoir beaucoup de type différents</t>
   </si>
 </sst>
 </file>
@@ -1202,12 +1156,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1219,16 +1173,16 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>3</v>
@@ -1237,49 +1191,49 @@
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="K6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="Q8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="Q9" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
@@ -1290,103 +1244,103 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M10" s="2"/>
       <c r="Q10" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="S10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="T10" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="T10" s="10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="Q13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
@@ -1396,44 +1350,44 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="U19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
@@ -1442,20 +1396,20 @@
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1469,36 +1423,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28BBB61-DFBD-4DBE-8C12-2C1BEFFE2DFA}">
   <dimension ref="B2:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="6" max="6" width="8.21875" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
@@ -1507,53 +1464,53 @@
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
@@ -1561,7 +1518,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -1569,192 +1526,192 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="L36" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1768,23 +1725,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F477EC8-D57D-4BB2-99A4-02D9F3FFB1AD}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1792,164 +1749,74 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I8" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF4BCD2-0275-40CE-94FA-6A4F0B5C146F}">
-  <dimension ref="C6:C31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modelisation : renamed tables and attributes + added tables Awards, Review ann festivals. Documentation : added some questions and answers from a teacher + added some explanations for some of the tables and their attributes
</commit_message>
<xml_diff>
--- a/Documentation/database-tables.xlsx
+++ b/Documentation/database-tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clem\01-coding-projects\08-sql-projects\projet-bdd-2021\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6861F8A1-7EBC-4D0A-BD78-08D7D0C9F5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D9D1A2-29C4-4211-A7B6-4E2EF834DA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D0EBE73F-8EE6-4ABE-837B-C7604514A6B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D0EBE73F-8EE6-4ABE-837B-C7604514A6B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Modélisation" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="116">
   <si>
     <t>BDD</t>
   </si>
@@ -387,9 +387,6 @@
     <t>pas d'accent</t>
   </si>
   <si>
-    <t>pas d'espace, seulement des underscores _</t>
-  </si>
-  <si>
     <t>musicienne, comedienne, realisatrice, metteuse en scene, scénariste/autrice</t>
   </si>
   <si>
@@ -408,9 +405,6 @@
     <t>nom au singulier</t>
   </si>
   <si>
-    <t>table de liaison : nom des 2 tables separes par un underscore _</t>
-  </si>
-  <si>
     <t>Règles de nommage</t>
   </si>
   <si>
@@ -648,9 +642,6 @@
     <t>anglais</t>
   </si>
   <si>
-    <t>commits commencent par : feature, bug fix, enhancement, documentation</t>
-  </si>
-  <si>
     <t>agency_payment</t>
   </si>
   <si>
@@ -682,6 +673,24 @@
   </si>
   <si>
     <t>text contenant prix, date, œuvre, etc.</t>
+  </si>
+  <si>
+    <t>Premiere lette en majuscule</t>
+  </si>
+  <si>
+    <t>tout en minuscule</t>
+  </si>
+  <si>
+    <t>separation des mots avec des underscores _</t>
+  </si>
+  <si>
+    <t>pas d'espace et de caracteres speciaux, seulement des underscores _ (et *)</t>
+  </si>
+  <si>
+    <t>commits commencent par : modelisation, feature, bug fix, enhancement, documentation</t>
+  </si>
+  <si>
+    <t>Separation entre mots grâce à des majuscules</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88356EE-5369-4008-B71C-3EFE3FF6D012}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -1156,12 +1165,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1173,16 +1182,16 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>3</v>
@@ -1191,22 +1200,22 @@
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="K6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>9</v>
@@ -1214,26 +1223,26 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="Q8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="Q9" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
@@ -1244,26 +1253,26 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M10" s="2"/>
       <c r="Q10" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="S10" s="10" t="s">
         <v>7</v>
@@ -1274,56 +1283,56 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="Q13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>9</v>
@@ -1334,10 +1343,10 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R15" t="s">
         <v>10</v>
@@ -1350,24 +1359,24 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>8</v>
@@ -1376,7 +1385,7 @@
         <v>7</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U18" s="3" t="s">
         <v>11</v>
@@ -1384,7 +1393,7 @@
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U19" t="s">
         <v>12</v>
@@ -1396,20 +1405,20 @@
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1423,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28BBB61-DFBD-4DBE-8C12-2C1BEFFE2DFA}">
   <dimension ref="B2:O42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1441,21 +1450,21 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
@@ -1464,53 +1473,53 @@
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
@@ -1518,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -1526,189 +1535,189 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="L36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M42" s="1" t="s">
         <v>7</v>
@@ -1725,23 +1734,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F477EC8-D57D-4BB2-99A4-02D9F3FFB1AD}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1749,7 +1758,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1757,52 +1766,65 @@
         <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>113</v>
+      </c>
+      <c r="I6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I9" t="s">
-        <v>20</v>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K15" t="s">
+        <v>103</v>
+      </c>
+      <c r="M15" t="s">
         <v>106</v>
-      </c>
-      <c r="M15" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1812,7 +1834,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>